<commit_message>
improved excel result sheet
</commit_message>
<xml_diff>
--- a/output/results_Excel.xlsx
+++ b/output/results_Excel.xlsx
@@ -214,6 +214,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -235,14 +236,21 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66CC00"/>
+        <bgColor rgb="FF339966"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -284,8 +292,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -297,6 +305,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF66CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -308,19 +376,19 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4540816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8826530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.280612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.8112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.234693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.9285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>